<commit_message>
new selector prev month
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D41683A-70C1-475F-AC1F-523018343F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429F0ECA-6AE5-49EE-9471-BB9843E1F4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="990" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,7 +365,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44789</v>
+        <v>43831</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -373,7 +373,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>44895</v>
+        <v>43846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working with any range of calendar dates
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\bot4\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429F0ECA-6AE5-49EE-9471-BB9843E1F4B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEDF46A-DDAD-4EFE-9F6E-31D6A2EEB0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="990" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>43831</v>
+        <v>44103</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -373,7 +373,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>43846</v>
+        <v>44210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>